<commit_message>
[IMP] 使用optional替换if (xxx == null)
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-03-27-init-data.xlsx
+++ b/src/main/resources/script/db/2018-03-27-init-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19770" windowHeight="9375" tabRatio="987" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19770" windowHeight="9375" tabRatio="987" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="195">
   <si>
     <r>
       <rPr>
@@ -2461,6 +2461,26 @@
   </si>
   <si>
     <t>http://localhost:9090</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>organization administrator</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>project administrator</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>project owner</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>project owner</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>project member</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -4287,8 +4307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D7:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -4319,9 +4339,8 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="4:9">
-      <c r="E8" t="str">
-        <f>iam_role!E8</f>
-        <v>role/site/default/administrator</v>
+      <c r="E8" t="s">
+        <v>190</v>
       </c>
       <c r="F8" t="str">
         <f>iam_role!E9</f>
@@ -4333,9 +4352,8 @@
       </c>
     </row>
     <row r="9" spans="4:9">
-      <c r="E9" t="str">
-        <f>iam_role!E9</f>
-        <v>role/orgainzation/default/administrator</v>
+      <c r="E9" t="s">
+        <v>191</v>
       </c>
       <c r="F9" t="str">
         <f>iam_role!E10</f>
@@ -4347,9 +4365,8 @@
       </c>
     </row>
     <row r="10" spans="4:9">
-      <c r="E10" t="str">
-        <f>iam_role!E13</f>
-        <v>role/project/default/project-owner</v>
+      <c r="E10" t="s">
+        <v>192</v>
       </c>
       <c r="F10" t="str">
         <f>iam_role!E13</f>
@@ -4361,9 +4378,8 @@
       </c>
     </row>
     <row r="11" spans="4:9">
-      <c r="E11" t="str">
-        <f>iam_role!E13</f>
-        <v>role/project/default/project-owner</v>
+      <c r="E11" t="s">
+        <v>193</v>
       </c>
       <c r="F11" t="str">
         <f>iam_role!E13</f>
@@ -4375,9 +4391,8 @@
       </c>
     </row>
     <row r="12" spans="4:9">
-      <c r="E12" t="str">
-        <f>iam_role!E12</f>
-        <v>role/project/default/project-member</v>
+      <c r="E12" t="s">
+        <v>194</v>
       </c>
       <c r="F12" t="str">
         <f>iam_role!E12</f>
@@ -4642,7 +4657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[FIX] fix xlsx error
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-03-27-init-data.xlsx
+++ b/src/main/resources/script/db/2018-03-27-init-data.xlsx
@@ -4383,8 +4383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -5050,7 +5050,7 @@
   <dimension ref="D7:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -5141,7 +5141,7 @@
         <v>role/site/default/developer</v>
       </c>
       <c r="F10" t="str">
-        <f>iam_role!F15</f>
+        <f>iam_role!E15</f>
         <v>role/site/default/developer</v>
       </c>
       <c r="G10" t="str">

</xml_diff>

<commit_message>
[ADD] init-data-xlsx add site wiki admin label and role.
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-03-27-init-data.xlsx
+++ b/src/main/resources/script/db/2018-03-27-init-data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\idea_work_workspace\gitlab\framework-group\iam-service\src\main\resources\script\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DYQ\tranning\choerodon-framework\iam-service\src\main\resources\script\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C14F48-9CB7-4236-84BF-990D588D33C8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19770" windowHeight="9375" tabRatio="987" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19770" windowHeight="9375" tabRatio="987" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -30,12 +31,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">README!$D$1:$D$4</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="252">
   <si>
     <r>
       <rPr>
@@ -2696,13 +2697,32 @@
   </si>
   <si>
     <t>OpenLDAP</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>site.wiki.admin</t>
+  </si>
+  <si>
+    <t>site.wiki.admin</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>site</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>全局层wiki管理员</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>site wiki admin</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m/d/yyyy"/>
   </numFmts>
@@ -3140,7 +3160,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="1"/>
+    <cellStyle name="Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="2" builtinId="8"/>
   </cellStyles>
@@ -3482,7 +3502,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView topLeftCell="B4" workbookViewId="0">
@@ -3733,7 +3753,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="D7:I8"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
@@ -3790,7 +3810,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="D7:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3874,10 +3894,10 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="D7:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -3942,7 +3962,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="D7:N8"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -4038,7 +4058,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -4111,11 +4131,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D7:I17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="D7:I18"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4315,6 +4335,23 @@
         <v>160</v>
       </c>
     </row>
+    <row r="18" spans="5:9">
+      <c r="E18" t="s">
+        <v>248</v>
+      </c>
+      <c r="F18" t="s">
+        <v>247</v>
+      </c>
+      <c r="G18" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" t="s">
+        <v>249</v>
+      </c>
+      <c r="I18" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4322,7 +4359,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -4434,7 +4471,7 @@
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1"/>
+    <hyperlink ref="H8" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.69791666666666696" right="0.69791666666666696" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -4442,11 +4479,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B7:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -4770,11 +4807,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D7:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="D7:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -4962,6 +4999,19 @@
         <v>project.owner</v>
       </c>
     </row>
+    <row r="20" spans="5:7">
+      <c r="E20" t="s">
+        <v>251</v>
+      </c>
+      <c r="F20" t="str">
+        <f>IAM_ROLE!E8</f>
+        <v>role/site/default/administrator</v>
+      </c>
+      <c r="G20" t="str">
+        <f>IAM_LABEL!E18</f>
+        <v>site.wiki.admin</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4970,7 +5020,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5110,7 +5160,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="D7:J10"/>
   <sheetViews>
     <sheetView topLeftCell="C2" workbookViewId="0">
@@ -5234,7 +5284,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
[FIX] init-data.xlsx update site.wiki.admin to site.admin
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/2018-03-27-init-data.xlsx
+++ b/src/main/resources/script/db/2018-03-27-init-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DYQ\tranning\choerodon-framework\iam-service\src\main\resources\script\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C14F48-9CB7-4236-84BF-990D588D33C8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9389CBEA-9B30-4185-8465-6A6E08C059CD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19770" windowHeight="9375" tabRatio="987" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2700,22 +2700,23 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>site.wiki.admin</t>
-  </si>
-  <si>
-    <t>site.wiki.admin</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
     <t>site</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>全局层wiki管理员</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>site wiki admin</t>
+    <t>site.admin</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>site.admin</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>全局层管理员</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>site admin</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -4135,7 +4136,7 @@
   <dimension ref="D7:I18"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4340,13 +4341,13 @@
         <v>248</v>
       </c>
       <c r="F18" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="G18" t="s">
         <v>78</v>
       </c>
       <c r="H18" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I18" t="s">
         <v>250</v>
@@ -5009,7 +5010,7 @@
       </c>
       <c r="G20" t="str">
         <f>IAM_LABEL!E18</f>
-        <v>site.wiki.admin</v>
+        <v>site.admin</v>
       </c>
     </row>
   </sheetData>

</xml_diff>